<commit_message>
Revert "defines heavy armor"
This reverts commit ffbe49040d5ce26b3fdea2445eea5da3e57dd007.
</commit_message>
<xml_diff>
--- a/resources/Equipment stats.xlsx
+++ b/resources/Equipment stats.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA68F021-1160-47F5-93DA-67BBA279BAF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32D58957-E235-4A61-837C-474BFB14F1E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="1935" windowWidth="23820" windowHeight="12810" xr2:uid="{3B1F7097-C083-41C8-BF05-DD0840C0153C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B1F7097-C083-41C8-BF05-DD0840C0153C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -716,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687D9CB0-23D6-49DF-92B5-545D181FEEE3}">
   <dimension ref="D2:AI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L92" sqref="L92"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,7 +2789,7 @@
         <v>30</v>
       </c>
       <c r="M62">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N62">
         <v>60</v>
@@ -2798,7 +2799,7 @@
       </c>
       <c r="P62">
         <f>M62*N62/O62/10</f>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q62">
         <v>3</v>
@@ -2884,7 +2885,7 @@
         <v>50</v>
       </c>
       <c r="M63">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N63">
         <v>60</v>
@@ -2894,7 +2895,7 @@
       </c>
       <c r="P63">
         <f t="shared" ref="P63:P90" si="11">M63*N63/O63/10</f>
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q63">
         <v>4</v>
@@ -2913,7 +2914,7 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="V63">
-        <f t="shared" ref="V63:X63" si="12">F63/F62</f>
+        <f t="shared" ref="V62:X63" si="12">F63/F62</f>
         <v>1.2</v>
       </c>
       <c r="W63">
@@ -2925,43 +2926,43 @@
         <v>2</v>
       </c>
       <c r="Y63">
-        <f t="shared" ref="Y63" si="13">I63/I62</f>
+        <f t="shared" ref="Y62:Y63" si="13">I63/I62</f>
         <v>1.2857142857142858</v>
       </c>
       <c r="Z63">
-        <f t="shared" ref="Z63" si="14">J63/J62</f>
+        <f t="shared" ref="Z62:Z63" si="14">J63/J62</f>
         <v>1.5</v>
       </c>
       <c r="AB63">
-        <f t="shared" ref="AB63" si="15">L63/L62</f>
+        <f t="shared" ref="AB62:AB63" si="15">L63/L62</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="AC63">
-        <f t="shared" ref="AC63" si="16">M63/M62</f>
-        <v>1.0909090909090908</v>
+        <f t="shared" ref="AC62:AC63" si="16">M63/M62</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AD63">
-        <f t="shared" ref="AD63" si="17">N63/N62</f>
+        <f t="shared" ref="AD62:AD63" si="17">N63/N62</f>
         <v>1</v>
       </c>
       <c r="AE63">
-        <f t="shared" ref="AE63" si="18">O63/O62</f>
+        <f t="shared" ref="AE62:AE63" si="18">O63/O62</f>
         <v>1</v>
       </c>
       <c r="AF63">
         <f>P63/P62</f>
-        <v>1.0909090909090908</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AG63">
-        <f t="shared" ref="AG63" si="19">Q63/Q62</f>
+        <f t="shared" ref="AG62:AG63" si="19">Q63/Q62</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="AH63" t="e">
-        <f t="shared" ref="AH63" si="20">R63/R62</f>
+        <f t="shared" ref="AH62:AH63" si="20">R63/R62</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AI63" t="e">
-        <f t="shared" ref="AI63" si="21">S63/S62</f>
+        <f t="shared" ref="AI62:AI63" si="21">S63/S62</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3115,59 +3116,59 @@
         <v>86</v>
       </c>
       <c r="U65">
-        <f t="shared" ref="U65:U90" si="22">E65/E64</f>
+        <f t="shared" ref="U64:U90" si="22">E65/E64</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="V65">
-        <f t="shared" ref="V65:V90" si="23">F65/F64</f>
+        <f t="shared" ref="V64:V90" si="23">F65/F64</f>
         <v>1.4</v>
       </c>
       <c r="W65">
-        <f t="shared" ref="W65:W90" si="24">G65/G64</f>
+        <f t="shared" ref="W64:W90" si="24">G65/G64</f>
         <v>1.4</v>
       </c>
       <c r="X65">
-        <f t="shared" ref="X65:X90" si="25">H65/H64</f>
+        <f t="shared" ref="X64:X90" si="25">H65/H64</f>
         <v>2.5</v>
       </c>
       <c r="Y65">
-        <f t="shared" ref="Y65:Y90" si="26">I65/I64</f>
+        <f t="shared" ref="Y64:Y90" si="26">I65/I64</f>
         <v>1.125</v>
       </c>
       <c r="Z65">
-        <f t="shared" ref="Z65:Z90" si="27">J65/J64</f>
+        <f t="shared" ref="Z64:Z90" si="27">J65/J64</f>
         <v>1.5</v>
       </c>
       <c r="AB65">
-        <f t="shared" ref="AB65:AB90" si="28">L65/L64</f>
+        <f t="shared" ref="AB64:AB90" si="28">L65/L64</f>
         <v>1</v>
       </c>
       <c r="AC65">
-        <f t="shared" ref="AC65:AC90" si="29">M65/M64</f>
+        <f t="shared" ref="AC64:AC90" si="29">M65/M64</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AD65">
-        <f t="shared" ref="AD65:AD90" si="30">N65/N64</f>
+        <f t="shared" ref="AD64:AD90" si="30">N65/N64</f>
         <v>1</v>
       </c>
       <c r="AE65">
-        <f t="shared" ref="AE65:AE90" si="31">O65/O64</f>
+        <f t="shared" ref="AE64:AE90" si="31">O65/O64</f>
         <v>1</v>
       </c>
       <c r="AF65">
-        <f t="shared" ref="AF65:AF90" si="32">P65/P64</f>
+        <f t="shared" ref="AF64:AF90" si="32">P65/P64</f>
         <v>1.0999999999999999</v>
       </c>
       <c r="AG65">
-        <f t="shared" ref="AG65:AG90" si="33">Q65/Q64</f>
+        <f t="shared" ref="AG64:AG90" si="33">Q65/Q64</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="AH65">
-        <f t="shared" ref="AH65:AH90" si="34">R65/R64</f>
+        <f t="shared" ref="AH64:AH90" si="34">R65/R64</f>
         <v>1</v>
       </c>
       <c r="AI65" t="e">
-        <f t="shared" ref="AI65:AI90" si="35">S65/S64</f>
+        <f t="shared" ref="AI64:AI90" si="35">S65/S64</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3554,7 +3555,7 @@
         <v>2.6666666666666665</v>
       </c>
       <c r="AA69">
-        <f t="shared" ref="AA69:AA81" si="36">K69/K68</f>
+        <f t="shared" ref="AA64:AA90" si="36">K69/K68</f>
         <v>1.1764705882352942</v>
       </c>
       <c r="AB69">
@@ -3619,7 +3620,7 @@
         <v>71</v>
       </c>
       <c r="M70" s="2">
-        <v>14.5</v>
+        <v>13.5</v>
       </c>
       <c r="N70">
         <v>50</v>
@@ -3629,7 +3630,7 @@
       </c>
       <c r="P70">
         <f t="shared" si="11"/>
-        <v>36.25</v>
+        <v>33.75</v>
       </c>
       <c r="Q70">
         <v>2</v>
@@ -3715,7 +3716,7 @@
         <v>81</v>
       </c>
       <c r="M71">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N71">
         <v>50</v>
@@ -3725,7 +3726,7 @@
       </c>
       <c r="P71">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>37.5</v>
       </c>
       <c r="Q71">
         <v>3</v>
@@ -3769,7 +3770,7 @@
       </c>
       <c r="AC71">
         <f t="shared" si="29"/>
-        <v>1.103448275862069</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="AD71">
         <f t="shared" si="30"/>
@@ -3781,7 +3782,7 @@
       </c>
       <c r="AF71">
         <f t="shared" si="32"/>
-        <v>1.103448275862069</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="AG71">
         <f t="shared" si="33"/>
@@ -3825,7 +3826,7 @@
         <v>95</v>
       </c>
       <c r="M72">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N72">
         <v>50</v>
@@ -3835,7 +3836,7 @@
       </c>
       <c r="P72">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>37.5</v>
       </c>
       <c r="Q72">
         <v>3</v>
@@ -4894,7 +4895,7 @@
         <v>90</v>
       </c>
       <c r="M82" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N82">
         <v>40</v>
@@ -4904,7 +4905,7 @@
       </c>
       <c r="P82">
         <f t="shared" si="11"/>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q82">
         <v>3</v>
@@ -4990,7 +4991,7 @@
         <v>111</v>
       </c>
       <c r="M83">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N83">
         <v>40</v>
@@ -5000,7 +5001,7 @@
       </c>
       <c r="P83">
         <f t="shared" si="11"/>
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q83">
         <v>3</v>
@@ -5044,7 +5045,7 @@
       </c>
       <c r="AC83">
         <f t="shared" si="29"/>
-        <v>1.1379310344827587</v>
+        <v>1.1428571428571428</v>
       </c>
       <c r="AD83">
         <f t="shared" si="30"/>
@@ -5056,7 +5057,7 @@
       </c>
       <c r="AF83">
         <f t="shared" si="32"/>
-        <v>1.1379310344827587</v>
+        <v>1.1428571428571428</v>
       </c>
       <c r="AG83">
         <f t="shared" si="33"/>
@@ -5100,7 +5101,7 @@
         <v>131</v>
       </c>
       <c r="M84" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N84">
         <v>40</v>
@@ -5110,7 +5111,7 @@
       </c>
       <c r="P84">
         <f t="shared" si="11"/>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q84">
         <v>4</v>
@@ -5154,7 +5155,7 @@
       </c>
       <c r="AC84">
         <f t="shared" si="29"/>
-        <v>1.0909090909090908</v>
+        <v>1.09375</v>
       </c>
       <c r="AD84">
         <f t="shared" si="30"/>
@@ -5166,7 +5167,7 @@
       </c>
       <c r="AF84">
         <f t="shared" si="32"/>
-        <v>1.0909090909090908</v>
+        <v>1.09375</v>
       </c>
       <c r="AG84">
         <f t="shared" si="33"/>

</xml_diff>

<commit_message>
Revert "Revert "defines heavy armor""
This reverts commit ec99ee0df2bc9edd16f11469a622519c5a7b77e4.
</commit_message>
<xml_diff>
--- a/resources/Equipment stats.xlsx
+++ b/resources/Equipment stats.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32D58957-E235-4A61-837C-474BFB14F1E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA68F021-1160-47F5-93DA-67BBA279BAF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B1F7097-C083-41C8-BF05-DD0840C0153C}"/>
+    <workbookView xWindow="3030" yWindow="1935" windowWidth="23820" windowHeight="12810" xr2:uid="{3B1F7097-C083-41C8-BF05-DD0840C0153C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -717,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687D9CB0-23D6-49DF-92B5-545D181FEEE3}">
   <dimension ref="D2:AI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,7 +2788,7 @@
         <v>30</v>
       </c>
       <c r="M62">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N62">
         <v>60</v>
@@ -2799,7 +2798,7 @@
       </c>
       <c r="P62">
         <f>M62*N62/O62/10</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q62">
         <v>3</v>
@@ -2885,7 +2884,7 @@
         <v>50</v>
       </c>
       <c r="M63">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N63">
         <v>60</v>
@@ -2895,7 +2894,7 @@
       </c>
       <c r="P63">
         <f t="shared" ref="P63:P90" si="11">M63*N63/O63/10</f>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q63">
         <v>4</v>
@@ -2914,7 +2913,7 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="V63">
-        <f t="shared" ref="V62:X63" si="12">F63/F62</f>
+        <f t="shared" ref="V63:X63" si="12">F63/F62</f>
         <v>1.2</v>
       </c>
       <c r="W63">
@@ -2926,43 +2925,43 @@
         <v>2</v>
       </c>
       <c r="Y63">
-        <f t="shared" ref="Y62:Y63" si="13">I63/I62</f>
+        <f t="shared" ref="Y63" si="13">I63/I62</f>
         <v>1.2857142857142858</v>
       </c>
       <c r="Z63">
-        <f t="shared" ref="Z62:Z63" si="14">J63/J62</f>
+        <f t="shared" ref="Z63" si="14">J63/J62</f>
         <v>1.5</v>
       </c>
       <c r="AB63">
-        <f t="shared" ref="AB62:AB63" si="15">L63/L62</f>
+        <f t="shared" ref="AB63" si="15">L63/L62</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="AC63">
-        <f t="shared" ref="AC62:AC63" si="16">M63/M62</f>
-        <v>1.1000000000000001</v>
+        <f t="shared" ref="AC63" si="16">M63/M62</f>
+        <v>1.0909090909090908</v>
       </c>
       <c r="AD63">
-        <f t="shared" ref="AD62:AD63" si="17">N63/N62</f>
+        <f t="shared" ref="AD63" si="17">N63/N62</f>
         <v>1</v>
       </c>
       <c r="AE63">
-        <f t="shared" ref="AE62:AE63" si="18">O63/O62</f>
+        <f t="shared" ref="AE63" si="18">O63/O62</f>
         <v>1</v>
       </c>
       <c r="AF63">
         <f>P63/P62</f>
-        <v>1.1000000000000001</v>
+        <v>1.0909090909090908</v>
       </c>
       <c r="AG63">
-        <f t="shared" ref="AG62:AG63" si="19">Q63/Q62</f>
+        <f t="shared" ref="AG63" si="19">Q63/Q62</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="AH63" t="e">
-        <f t="shared" ref="AH62:AH63" si="20">R63/R62</f>
+        <f t="shared" ref="AH63" si="20">R63/R62</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AI63" t="e">
-        <f t="shared" ref="AI62:AI63" si="21">S63/S62</f>
+        <f t="shared" ref="AI63" si="21">S63/S62</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3116,59 +3115,59 @@
         <v>86</v>
       </c>
       <c r="U65">
-        <f t="shared" ref="U64:U90" si="22">E65/E64</f>
+        <f t="shared" ref="U65:U90" si="22">E65/E64</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="V65">
-        <f t="shared" ref="V64:V90" si="23">F65/F64</f>
+        <f t="shared" ref="V65:V90" si="23">F65/F64</f>
         <v>1.4</v>
       </c>
       <c r="W65">
-        <f t="shared" ref="W64:W90" si="24">G65/G64</f>
+        <f t="shared" ref="W65:W90" si="24">G65/G64</f>
         <v>1.4</v>
       </c>
       <c r="X65">
-        <f t="shared" ref="X64:X90" si="25">H65/H64</f>
+        <f t="shared" ref="X65:X90" si="25">H65/H64</f>
         <v>2.5</v>
       </c>
       <c r="Y65">
-        <f t="shared" ref="Y64:Y90" si="26">I65/I64</f>
+        <f t="shared" ref="Y65:Y90" si="26">I65/I64</f>
         <v>1.125</v>
       </c>
       <c r="Z65">
-        <f t="shared" ref="Z64:Z90" si="27">J65/J64</f>
+        <f t="shared" ref="Z65:Z90" si="27">J65/J64</f>
         <v>1.5</v>
       </c>
       <c r="AB65">
-        <f t="shared" ref="AB64:AB90" si="28">L65/L64</f>
+        <f t="shared" ref="AB65:AB90" si="28">L65/L64</f>
         <v>1</v>
       </c>
       <c r="AC65">
-        <f t="shared" ref="AC64:AC90" si="29">M65/M64</f>
+        <f t="shared" ref="AC65:AC90" si="29">M65/M64</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AD65">
-        <f t="shared" ref="AD64:AD90" si="30">N65/N64</f>
+        <f t="shared" ref="AD65:AD90" si="30">N65/N64</f>
         <v>1</v>
       </c>
       <c r="AE65">
-        <f t="shared" ref="AE64:AE90" si="31">O65/O64</f>
+        <f t="shared" ref="AE65:AE90" si="31">O65/O64</f>
         <v>1</v>
       </c>
       <c r="AF65">
-        <f t="shared" ref="AF64:AF90" si="32">P65/P64</f>
+        <f t="shared" ref="AF65:AF90" si="32">P65/P64</f>
         <v>1.0999999999999999</v>
       </c>
       <c r="AG65">
-        <f t="shared" ref="AG64:AG90" si="33">Q65/Q64</f>
+        <f t="shared" ref="AG65:AG90" si="33">Q65/Q64</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="AH65">
-        <f t="shared" ref="AH64:AH90" si="34">R65/R64</f>
+        <f t="shared" ref="AH65:AH90" si="34">R65/R64</f>
         <v>1</v>
       </c>
       <c r="AI65" t="e">
-        <f t="shared" ref="AI64:AI90" si="35">S65/S64</f>
+        <f t="shared" ref="AI65:AI90" si="35">S65/S64</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3555,7 +3554,7 @@
         <v>2.6666666666666665</v>
       </c>
       <c r="AA69">
-        <f t="shared" ref="AA64:AA90" si="36">K69/K68</f>
+        <f t="shared" ref="AA69:AA81" si="36">K69/K68</f>
         <v>1.1764705882352942</v>
       </c>
       <c r="AB69">
@@ -3620,7 +3619,7 @@
         <v>71</v>
       </c>
       <c r="M70" s="2">
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
       <c r="N70">
         <v>50</v>
@@ -3630,7 +3629,7 @@
       </c>
       <c r="P70">
         <f t="shared" si="11"/>
-        <v>33.75</v>
+        <v>36.25</v>
       </c>
       <c r="Q70">
         <v>2</v>
@@ -3716,7 +3715,7 @@
         <v>81</v>
       </c>
       <c r="M71">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N71">
         <v>50</v>
@@ -3726,7 +3725,7 @@
       </c>
       <c r="P71">
         <f t="shared" si="11"/>
-        <v>37.5</v>
+        <v>40</v>
       </c>
       <c r="Q71">
         <v>3</v>
@@ -3770,7 +3769,7 @@
       </c>
       <c r="AC71">
         <f t="shared" si="29"/>
-        <v>1.1111111111111112</v>
+        <v>1.103448275862069</v>
       </c>
       <c r="AD71">
         <f t="shared" si="30"/>
@@ -3782,7 +3781,7 @@
       </c>
       <c r="AF71">
         <f t="shared" si="32"/>
-        <v>1.1111111111111112</v>
+        <v>1.103448275862069</v>
       </c>
       <c r="AG71">
         <f t="shared" si="33"/>
@@ -3826,7 +3825,7 @@
         <v>95</v>
       </c>
       <c r="M72">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N72">
         <v>50</v>
@@ -3836,7 +3835,7 @@
       </c>
       <c r="P72">
         <f t="shared" si="11"/>
-        <v>37.5</v>
+        <v>40</v>
       </c>
       <c r="Q72">
         <v>3</v>
@@ -4895,7 +4894,7 @@
         <v>90</v>
       </c>
       <c r="M82" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N82">
         <v>40</v>
@@ -4905,7 +4904,7 @@
       </c>
       <c r="P82">
         <f t="shared" si="11"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q82">
         <v>3</v>
@@ -4991,7 +4990,7 @@
         <v>111</v>
       </c>
       <c r="M83">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N83">
         <v>40</v>
@@ -5001,7 +5000,7 @@
       </c>
       <c r="P83">
         <f t="shared" si="11"/>
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q83">
         <v>3</v>
@@ -5045,7 +5044,7 @@
       </c>
       <c r="AC83">
         <f t="shared" si="29"/>
-        <v>1.1428571428571428</v>
+        <v>1.1379310344827587</v>
       </c>
       <c r="AD83">
         <f t="shared" si="30"/>
@@ -5057,7 +5056,7 @@
       </c>
       <c r="AF83">
         <f t="shared" si="32"/>
-        <v>1.1428571428571428</v>
+        <v>1.1379310344827587</v>
       </c>
       <c r="AG83">
         <f t="shared" si="33"/>
@@ -5101,7 +5100,7 @@
         <v>131</v>
       </c>
       <c r="M84" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N84">
         <v>40</v>
@@ -5111,7 +5110,7 @@
       </c>
       <c r="P84">
         <f t="shared" si="11"/>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Q84">
         <v>4</v>
@@ -5155,7 +5154,7 @@
       </c>
       <c r="AC84">
         <f t="shared" si="29"/>
-        <v>1.09375</v>
+        <v>1.0909090909090908</v>
       </c>
       <c r="AD84">
         <f t="shared" si="30"/>
@@ -5167,7 +5166,7 @@
       </c>
       <c r="AF84">
         <f t="shared" si="32"/>
-        <v>1.09375</v>
+        <v>1.0909090909090908</v>
       </c>
       <c r="AG84">
         <f t="shared" si="33"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "defines heavy armor"""
This reverts commit 5e89ee39596cfa8b8ff1b9cad8f0ce7801eb27f6.
</commit_message>
<xml_diff>
--- a/resources/Equipment stats.xlsx
+++ b/resources/Equipment stats.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA68F021-1160-47F5-93DA-67BBA279BAF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32D58957-E235-4A61-837C-474BFB14F1E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="1935" windowWidth="23820" windowHeight="12810" xr2:uid="{3B1F7097-C083-41C8-BF05-DD0840C0153C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B1F7097-C083-41C8-BF05-DD0840C0153C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -716,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687D9CB0-23D6-49DF-92B5-545D181FEEE3}">
   <dimension ref="D2:AI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L92" sqref="L92"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,7 +2789,7 @@
         <v>30</v>
       </c>
       <c r="M62">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N62">
         <v>60</v>
@@ -2798,7 +2799,7 @@
       </c>
       <c r="P62">
         <f>M62*N62/O62/10</f>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q62">
         <v>3</v>
@@ -2884,7 +2885,7 @@
         <v>50</v>
       </c>
       <c r="M63">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N63">
         <v>60</v>
@@ -2894,7 +2895,7 @@
       </c>
       <c r="P63">
         <f t="shared" ref="P63:P90" si="11">M63*N63/O63/10</f>
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q63">
         <v>4</v>
@@ -2913,7 +2914,7 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="V63">
-        <f t="shared" ref="V63:X63" si="12">F63/F62</f>
+        <f t="shared" ref="V62:X63" si="12">F63/F62</f>
         <v>1.2</v>
       </c>
       <c r="W63">
@@ -2925,43 +2926,43 @@
         <v>2</v>
       </c>
       <c r="Y63">
-        <f t="shared" ref="Y63" si="13">I63/I62</f>
+        <f t="shared" ref="Y62:Y63" si="13">I63/I62</f>
         <v>1.2857142857142858</v>
       </c>
       <c r="Z63">
-        <f t="shared" ref="Z63" si="14">J63/J62</f>
+        <f t="shared" ref="Z62:Z63" si="14">J63/J62</f>
         <v>1.5</v>
       </c>
       <c r="AB63">
-        <f t="shared" ref="AB63" si="15">L63/L62</f>
+        <f t="shared" ref="AB62:AB63" si="15">L63/L62</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="AC63">
-        <f t="shared" ref="AC63" si="16">M63/M62</f>
-        <v>1.0909090909090908</v>
+        <f t="shared" ref="AC62:AC63" si="16">M63/M62</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AD63">
-        <f t="shared" ref="AD63" si="17">N63/N62</f>
+        <f t="shared" ref="AD62:AD63" si="17">N63/N62</f>
         <v>1</v>
       </c>
       <c r="AE63">
-        <f t="shared" ref="AE63" si="18">O63/O62</f>
+        <f t="shared" ref="AE62:AE63" si="18">O63/O62</f>
         <v>1</v>
       </c>
       <c r="AF63">
         <f>P63/P62</f>
-        <v>1.0909090909090908</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AG63">
-        <f t="shared" ref="AG63" si="19">Q63/Q62</f>
+        <f t="shared" ref="AG62:AG63" si="19">Q63/Q62</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="AH63" t="e">
-        <f t="shared" ref="AH63" si="20">R63/R62</f>
+        <f t="shared" ref="AH62:AH63" si="20">R63/R62</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AI63" t="e">
-        <f t="shared" ref="AI63" si="21">S63/S62</f>
+        <f t="shared" ref="AI62:AI63" si="21">S63/S62</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3115,59 +3116,59 @@
         <v>86</v>
       </c>
       <c r="U65">
-        <f t="shared" ref="U65:U90" si="22">E65/E64</f>
+        <f t="shared" ref="U64:U90" si="22">E65/E64</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="V65">
-        <f t="shared" ref="V65:V90" si="23">F65/F64</f>
+        <f t="shared" ref="V64:V90" si="23">F65/F64</f>
         <v>1.4</v>
       </c>
       <c r="W65">
-        <f t="shared" ref="W65:W90" si="24">G65/G64</f>
+        <f t="shared" ref="W64:W90" si="24">G65/G64</f>
         <v>1.4</v>
       </c>
       <c r="X65">
-        <f t="shared" ref="X65:X90" si="25">H65/H64</f>
+        <f t="shared" ref="X64:X90" si="25">H65/H64</f>
         <v>2.5</v>
       </c>
       <c r="Y65">
-        <f t="shared" ref="Y65:Y90" si="26">I65/I64</f>
+        <f t="shared" ref="Y64:Y90" si="26">I65/I64</f>
         <v>1.125</v>
       </c>
       <c r="Z65">
-        <f t="shared" ref="Z65:Z90" si="27">J65/J64</f>
+        <f t="shared" ref="Z64:Z90" si="27">J65/J64</f>
         <v>1.5</v>
       </c>
       <c r="AB65">
-        <f t="shared" ref="AB65:AB90" si="28">L65/L64</f>
+        <f t="shared" ref="AB64:AB90" si="28">L65/L64</f>
         <v>1</v>
       </c>
       <c r="AC65">
-        <f t="shared" ref="AC65:AC90" si="29">M65/M64</f>
+        <f t="shared" ref="AC64:AC90" si="29">M65/M64</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AD65">
-        <f t="shared" ref="AD65:AD90" si="30">N65/N64</f>
+        <f t="shared" ref="AD64:AD90" si="30">N65/N64</f>
         <v>1</v>
       </c>
       <c r="AE65">
-        <f t="shared" ref="AE65:AE90" si="31">O65/O64</f>
+        <f t="shared" ref="AE64:AE90" si="31">O65/O64</f>
         <v>1</v>
       </c>
       <c r="AF65">
-        <f t="shared" ref="AF65:AF90" si="32">P65/P64</f>
+        <f t="shared" ref="AF64:AF90" si="32">P65/P64</f>
         <v>1.0999999999999999</v>
       </c>
       <c r="AG65">
-        <f t="shared" ref="AG65:AG90" si="33">Q65/Q64</f>
+        <f t="shared" ref="AG64:AG90" si="33">Q65/Q64</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="AH65">
-        <f t="shared" ref="AH65:AH90" si="34">R65/R64</f>
+        <f t="shared" ref="AH64:AH90" si="34">R65/R64</f>
         <v>1</v>
       </c>
       <c r="AI65" t="e">
-        <f t="shared" ref="AI65:AI90" si="35">S65/S64</f>
+        <f t="shared" ref="AI64:AI90" si="35">S65/S64</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3554,7 +3555,7 @@
         <v>2.6666666666666665</v>
       </c>
       <c r="AA69">
-        <f t="shared" ref="AA69:AA81" si="36">K69/K68</f>
+        <f t="shared" ref="AA64:AA90" si="36">K69/K68</f>
         <v>1.1764705882352942</v>
       </c>
       <c r="AB69">
@@ -3619,7 +3620,7 @@
         <v>71</v>
       </c>
       <c r="M70" s="2">
-        <v>14.5</v>
+        <v>13.5</v>
       </c>
       <c r="N70">
         <v>50</v>
@@ -3629,7 +3630,7 @@
       </c>
       <c r="P70">
         <f t="shared" si="11"/>
-        <v>36.25</v>
+        <v>33.75</v>
       </c>
       <c r="Q70">
         <v>2</v>
@@ -3715,7 +3716,7 @@
         <v>81</v>
       </c>
       <c r="M71">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N71">
         <v>50</v>
@@ -3725,7 +3726,7 @@
       </c>
       <c r="P71">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>37.5</v>
       </c>
       <c r="Q71">
         <v>3</v>
@@ -3769,7 +3770,7 @@
       </c>
       <c r="AC71">
         <f t="shared" si="29"/>
-        <v>1.103448275862069</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="AD71">
         <f t="shared" si="30"/>
@@ -3781,7 +3782,7 @@
       </c>
       <c r="AF71">
         <f t="shared" si="32"/>
-        <v>1.103448275862069</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="AG71">
         <f t="shared" si="33"/>
@@ -3825,7 +3826,7 @@
         <v>95</v>
       </c>
       <c r="M72">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N72">
         <v>50</v>
@@ -3835,7 +3836,7 @@
       </c>
       <c r="P72">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>37.5</v>
       </c>
       <c r="Q72">
         <v>3</v>
@@ -4894,7 +4895,7 @@
         <v>90</v>
       </c>
       <c r="M82" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N82">
         <v>40</v>
@@ -4904,7 +4905,7 @@
       </c>
       <c r="P82">
         <f t="shared" si="11"/>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q82">
         <v>3</v>
@@ -4990,7 +4991,7 @@
         <v>111</v>
       </c>
       <c r="M83">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N83">
         <v>40</v>
@@ -5000,7 +5001,7 @@
       </c>
       <c r="P83">
         <f t="shared" si="11"/>
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q83">
         <v>3</v>
@@ -5044,7 +5045,7 @@
       </c>
       <c r="AC83">
         <f t="shared" si="29"/>
-        <v>1.1379310344827587</v>
+        <v>1.1428571428571428</v>
       </c>
       <c r="AD83">
         <f t="shared" si="30"/>
@@ -5056,7 +5057,7 @@
       </c>
       <c r="AF83">
         <f t="shared" si="32"/>
-        <v>1.1379310344827587</v>
+        <v>1.1428571428571428</v>
       </c>
       <c r="AG83">
         <f t="shared" si="33"/>
@@ -5100,7 +5101,7 @@
         <v>131</v>
       </c>
       <c r="M84" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N84">
         <v>40</v>
@@ -5110,7 +5111,7 @@
       </c>
       <c r="P84">
         <f t="shared" si="11"/>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q84">
         <v>4</v>
@@ -5154,7 +5155,7 @@
       </c>
       <c r="AC84">
         <f t="shared" si="29"/>
-        <v>1.0909090909090908</v>
+        <v>1.09375</v>
       </c>
       <c r="AD84">
         <f t="shared" si="30"/>
@@ -5166,7 +5167,7 @@
       </c>
       <c r="AF84">
         <f t="shared" si="32"/>
-        <v>1.0909090909090908</v>
+        <v>1.09375</v>
       </c>
       <c r="AG84">
         <f t="shared" si="33"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "defines heavy armor""""
This reverts commit cc968ca7c90d2ed01badbda0d1680eb08337e411.
</commit_message>
<xml_diff>
--- a/resources/Equipment stats.xlsx
+++ b/resources/Equipment stats.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32D58957-E235-4A61-837C-474BFB14F1E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA68F021-1160-47F5-93DA-67BBA279BAF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B1F7097-C083-41C8-BF05-DD0840C0153C}"/>
+    <workbookView xWindow="3030" yWindow="1935" windowWidth="23820" windowHeight="12810" xr2:uid="{3B1F7097-C083-41C8-BF05-DD0840C0153C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -717,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687D9CB0-23D6-49DF-92B5-545D181FEEE3}">
   <dimension ref="D2:AI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,7 +2788,7 @@
         <v>30</v>
       </c>
       <c r="M62">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N62">
         <v>60</v>
@@ -2799,7 +2798,7 @@
       </c>
       <c r="P62">
         <f>M62*N62/O62/10</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q62">
         <v>3</v>
@@ -2885,7 +2884,7 @@
         <v>50</v>
       </c>
       <c r="M63">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N63">
         <v>60</v>
@@ -2895,7 +2894,7 @@
       </c>
       <c r="P63">
         <f t="shared" ref="P63:P90" si="11">M63*N63/O63/10</f>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q63">
         <v>4</v>
@@ -2914,7 +2913,7 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="V63">
-        <f t="shared" ref="V62:X63" si="12">F63/F62</f>
+        <f t="shared" ref="V63:X63" si="12">F63/F62</f>
         <v>1.2</v>
       </c>
       <c r="W63">
@@ -2926,43 +2925,43 @@
         <v>2</v>
       </c>
       <c r="Y63">
-        <f t="shared" ref="Y62:Y63" si="13">I63/I62</f>
+        <f t="shared" ref="Y63" si="13">I63/I62</f>
         <v>1.2857142857142858</v>
       </c>
       <c r="Z63">
-        <f t="shared" ref="Z62:Z63" si="14">J63/J62</f>
+        <f t="shared" ref="Z63" si="14">J63/J62</f>
         <v>1.5</v>
       </c>
       <c r="AB63">
-        <f t="shared" ref="AB62:AB63" si="15">L63/L62</f>
+        <f t="shared" ref="AB63" si="15">L63/L62</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="AC63">
-        <f t="shared" ref="AC62:AC63" si="16">M63/M62</f>
-        <v>1.1000000000000001</v>
+        <f t="shared" ref="AC63" si="16">M63/M62</f>
+        <v>1.0909090909090908</v>
       </c>
       <c r="AD63">
-        <f t="shared" ref="AD62:AD63" si="17">N63/N62</f>
+        <f t="shared" ref="AD63" si="17">N63/N62</f>
         <v>1</v>
       </c>
       <c r="AE63">
-        <f t="shared" ref="AE62:AE63" si="18">O63/O62</f>
+        <f t="shared" ref="AE63" si="18">O63/O62</f>
         <v>1</v>
       </c>
       <c r="AF63">
         <f>P63/P62</f>
-        <v>1.1000000000000001</v>
+        <v>1.0909090909090908</v>
       </c>
       <c r="AG63">
-        <f t="shared" ref="AG62:AG63" si="19">Q63/Q62</f>
+        <f t="shared" ref="AG63" si="19">Q63/Q62</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="AH63" t="e">
-        <f t="shared" ref="AH62:AH63" si="20">R63/R62</f>
+        <f t="shared" ref="AH63" si="20">R63/R62</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AI63" t="e">
-        <f t="shared" ref="AI62:AI63" si="21">S63/S62</f>
+        <f t="shared" ref="AI63" si="21">S63/S62</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3116,59 +3115,59 @@
         <v>86</v>
       </c>
       <c r="U65">
-        <f t="shared" ref="U64:U90" si="22">E65/E64</f>
+        <f t="shared" ref="U65:U90" si="22">E65/E64</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="V65">
-        <f t="shared" ref="V64:V90" si="23">F65/F64</f>
+        <f t="shared" ref="V65:V90" si="23">F65/F64</f>
         <v>1.4</v>
       </c>
       <c r="W65">
-        <f t="shared" ref="W64:W90" si="24">G65/G64</f>
+        <f t="shared" ref="W65:W90" si="24">G65/G64</f>
         <v>1.4</v>
       </c>
       <c r="X65">
-        <f t="shared" ref="X64:X90" si="25">H65/H64</f>
+        <f t="shared" ref="X65:X90" si="25">H65/H64</f>
         <v>2.5</v>
       </c>
       <c r="Y65">
-        <f t="shared" ref="Y64:Y90" si="26">I65/I64</f>
+        <f t="shared" ref="Y65:Y90" si="26">I65/I64</f>
         <v>1.125</v>
       </c>
       <c r="Z65">
-        <f t="shared" ref="Z64:Z90" si="27">J65/J64</f>
+        <f t="shared" ref="Z65:Z90" si="27">J65/J64</f>
         <v>1.5</v>
       </c>
       <c r="AB65">
-        <f t="shared" ref="AB64:AB90" si="28">L65/L64</f>
+        <f t="shared" ref="AB65:AB90" si="28">L65/L64</f>
         <v>1</v>
       </c>
       <c r="AC65">
-        <f t="shared" ref="AC64:AC90" si="29">M65/M64</f>
+        <f t="shared" ref="AC65:AC90" si="29">M65/M64</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AD65">
-        <f t="shared" ref="AD64:AD90" si="30">N65/N64</f>
+        <f t="shared" ref="AD65:AD90" si="30">N65/N64</f>
         <v>1</v>
       </c>
       <c r="AE65">
-        <f t="shared" ref="AE64:AE90" si="31">O65/O64</f>
+        <f t="shared" ref="AE65:AE90" si="31">O65/O64</f>
         <v>1</v>
       </c>
       <c r="AF65">
-        <f t="shared" ref="AF64:AF90" si="32">P65/P64</f>
+        <f t="shared" ref="AF65:AF90" si="32">P65/P64</f>
         <v>1.0999999999999999</v>
       </c>
       <c r="AG65">
-        <f t="shared" ref="AG64:AG90" si="33">Q65/Q64</f>
+        <f t="shared" ref="AG65:AG90" si="33">Q65/Q64</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="AH65">
-        <f t="shared" ref="AH64:AH90" si="34">R65/R64</f>
+        <f t="shared" ref="AH65:AH90" si="34">R65/R64</f>
         <v>1</v>
       </c>
       <c r="AI65" t="e">
-        <f t="shared" ref="AI64:AI90" si="35">S65/S64</f>
+        <f t="shared" ref="AI65:AI90" si="35">S65/S64</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3555,7 +3554,7 @@
         <v>2.6666666666666665</v>
       </c>
       <c r="AA69">
-        <f t="shared" ref="AA64:AA90" si="36">K69/K68</f>
+        <f t="shared" ref="AA69:AA81" si="36">K69/K68</f>
         <v>1.1764705882352942</v>
       </c>
       <c r="AB69">
@@ -3620,7 +3619,7 @@
         <v>71</v>
       </c>
       <c r="M70" s="2">
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
       <c r="N70">
         <v>50</v>
@@ -3630,7 +3629,7 @@
       </c>
       <c r="P70">
         <f t="shared" si="11"/>
-        <v>33.75</v>
+        <v>36.25</v>
       </c>
       <c r="Q70">
         <v>2</v>
@@ -3716,7 +3715,7 @@
         <v>81</v>
       </c>
       <c r="M71">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N71">
         <v>50</v>
@@ -3726,7 +3725,7 @@
       </c>
       <c r="P71">
         <f t="shared" si="11"/>
-        <v>37.5</v>
+        <v>40</v>
       </c>
       <c r="Q71">
         <v>3</v>
@@ -3770,7 +3769,7 @@
       </c>
       <c r="AC71">
         <f t="shared" si="29"/>
-        <v>1.1111111111111112</v>
+        <v>1.103448275862069</v>
       </c>
       <c r="AD71">
         <f t="shared" si="30"/>
@@ -3782,7 +3781,7 @@
       </c>
       <c r="AF71">
         <f t="shared" si="32"/>
-        <v>1.1111111111111112</v>
+        <v>1.103448275862069</v>
       </c>
       <c r="AG71">
         <f t="shared" si="33"/>
@@ -3826,7 +3825,7 @@
         <v>95</v>
       </c>
       <c r="M72">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N72">
         <v>50</v>
@@ -3836,7 +3835,7 @@
       </c>
       <c r="P72">
         <f t="shared" si="11"/>
-        <v>37.5</v>
+        <v>40</v>
       </c>
       <c r="Q72">
         <v>3</v>
@@ -4895,7 +4894,7 @@
         <v>90</v>
       </c>
       <c r="M82" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N82">
         <v>40</v>
@@ -4905,7 +4904,7 @@
       </c>
       <c r="P82">
         <f t="shared" si="11"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q82">
         <v>3</v>
@@ -4991,7 +4990,7 @@
         <v>111</v>
       </c>
       <c r="M83">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N83">
         <v>40</v>
@@ -5001,7 +5000,7 @@
       </c>
       <c r="P83">
         <f t="shared" si="11"/>
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q83">
         <v>3</v>
@@ -5045,7 +5044,7 @@
       </c>
       <c r="AC83">
         <f t="shared" si="29"/>
-        <v>1.1428571428571428</v>
+        <v>1.1379310344827587</v>
       </c>
       <c r="AD83">
         <f t="shared" si="30"/>
@@ -5057,7 +5056,7 @@
       </c>
       <c r="AF83">
         <f t="shared" si="32"/>
-        <v>1.1428571428571428</v>
+        <v>1.1379310344827587</v>
       </c>
       <c r="AG83">
         <f t="shared" si="33"/>
@@ -5101,7 +5100,7 @@
         <v>131</v>
       </c>
       <c r="M84" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N84">
         <v>40</v>
@@ -5111,7 +5110,7 @@
       </c>
       <c r="P84">
         <f t="shared" si="11"/>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Q84">
         <v>4</v>
@@ -5155,7 +5154,7 @@
       </c>
       <c r="AC84">
         <f t="shared" si="29"/>
-        <v>1.09375</v>
+        <v>1.0909090909090908</v>
       </c>
       <c r="AD84">
         <f t="shared" si="30"/>
@@ -5167,7 +5166,7 @@
       </c>
       <c r="AF84">
         <f t="shared" si="32"/>
-        <v>1.09375</v>
+        <v>1.0909090909090908</v>
       </c>
       <c r="AG84">
         <f t="shared" si="33"/>

</xml_diff>